<commit_message>
added more values to spreadsheet
</commit_message>
<xml_diff>
--- a/prog1_data.xlsx
+++ b/prog1_data.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emma/Documents/Spring 2016/CS 124/pset3/124pset3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16460" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
   <si>
     <t>Dimension</t>
   </si>
@@ -208,6 +213,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -533,22 +543,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Q31"/>
+  <dimension ref="A3:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="0.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1"/>
-    <row r="4" spans="1:17">
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -598,7 +608,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -624,7 +634,7 @@
         <v>2.1048170000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>3</v>
       </c>
@@ -650,7 +660,7 @@
         <v>1.4001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>4</v>
       </c>
@@ -676,7 +686,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>5</v>
       </c>
@@ -712,8 +722,8 @@
         <v>5.5259881066909836E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1"/>
-    <row r="10" spans="1:17">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>2</v>
       </c>
@@ -760,68 +770,93 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1"/>
-    <row r="13" spans="1:17">
-      <c r="C13">
+      <c r="E11">
+        <v>2.7233869999999998</v>
+      </c>
+      <c r="F11">
+        <v>3.8698130000000002</v>
+      </c>
+      <c r="G11">
+        <v>5.4370209999999997</v>
+      </c>
+      <c r="H11">
+        <v>7.6113479999999996</v>
+      </c>
+      <c r="I11">
+        <v>10.660026999999999</v>
+      </c>
+      <c r="J11">
+        <v>14.981488000000001</v>
+      </c>
+      <c r="K11">
+        <v>21.055610999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
         <v>3</v>
       </c>
+      <c r="E12">
+        <v>0.69535599999999997</v>
+      </c>
+      <c r="F12">
+        <v>0.44828499999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.352937</v>
+      </c>
+      <c r="H12">
+        <v>0.240012</v>
+      </c>
+      <c r="I12">
+        <v>0.184145</v>
+      </c>
+      <c r="J12">
+        <v>0.13089100000000001</v>
+      </c>
+      <c r="K12">
+        <v>8.2371E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>16</v>
+        <v>1000</v>
       </c>
       <c r="F13">
-        <v>32</v>
+        <v>1000</v>
       </c>
       <c r="G13">
-        <v>64</v>
+        <v>1000</v>
       </c>
       <c r="H13">
-        <v>128</v>
+        <v>1000</v>
       </c>
       <c r="I13">
-        <v>256</v>
+        <v>1000</v>
       </c>
       <c r="J13">
-        <v>512</v>
+        <v>1000</v>
       </c>
       <c r="K13">
-        <v>1024</v>
-      </c>
-      <c r="L13">
-        <v>2048</v>
-      </c>
-      <c r="M13">
-        <v>4096</v>
-      </c>
-      <c r="N13">
-        <v>8192</v>
-      </c>
-      <c r="O13">
-        <v>16834</v>
-      </c>
-      <c r="P13">
-        <v>32768</v>
-      </c>
-      <c r="Q13">
-        <v>65536</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1"/>
-    <row r="16" spans="1:17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
@@ -866,106 +901,310 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="4" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="E17">
+        <v>4.5239130000000003</v>
+      </c>
+      <c r="F17">
+        <v>7.1621389999999998</v>
+      </c>
+      <c r="G17">
+        <v>11.240602000000001</v>
+      </c>
+      <c r="H17">
+        <v>17.631734999999999</v>
+      </c>
+      <c r="I17">
+        <v>27.600925</v>
+      </c>
+      <c r="J17">
+        <v>43.319758999999998</v>
+      </c>
+      <c r="K17">
+        <v>68.157043000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>0.82371000000000005</v>
+      </c>
+      <c r="F18">
+        <v>0.72728199999999998</v>
+      </c>
+      <c r="G18">
+        <v>0.53383800000000003</v>
+      </c>
+      <c r="H18">
+        <v>0.43611</v>
+      </c>
+      <c r="I18">
+        <v>0.35639900000000002</v>
+      </c>
+      <c r="J18">
+        <v>0.25657000000000002</v>
+      </c>
+      <c r="K18">
+        <v>0.21005499999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>1000</v>
+      </c>
+      <c r="F19">
+        <v>1000</v>
+      </c>
+      <c r="G19">
+        <v>1000</v>
+      </c>
+      <c r="H19">
+        <v>1000</v>
+      </c>
+      <c r="I19">
+        <v>1000</v>
+      </c>
+      <c r="J19">
+        <v>1000</v>
+      </c>
+      <c r="K19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <v>32</v>
+      </c>
+      <c r="G22">
+        <v>64</v>
+      </c>
+      <c r="H22">
+        <v>128</v>
+      </c>
+      <c r="I22">
+        <v>256</v>
+      </c>
+      <c r="J22">
+        <v>512</v>
+      </c>
+      <c r="K22">
+        <v>1024</v>
+      </c>
+      <c r="L22">
+        <v>2048</v>
+      </c>
+      <c r="M22">
+        <v>4096</v>
+      </c>
+      <c r="N22">
+        <v>8192</v>
+      </c>
+      <c r="O22">
+        <v>16834</v>
+      </c>
+      <c r="P22">
+        <v>32768</v>
+      </c>
+      <c r="Q22">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>6.1359500000000002</v>
+      </c>
+      <c r="F23">
+        <v>10.339508</v>
+      </c>
+      <c r="G23">
+        <v>17.126459000000001</v>
+      </c>
+      <c r="H23">
+        <v>28.387136000000002</v>
+      </c>
+      <c r="I23">
+        <v>47.187328000000001</v>
+      </c>
+      <c r="J23">
+        <v>78.174957000000006</v>
+      </c>
+      <c r="K23">
+        <v>129.93571499999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>0.88619400000000004</v>
+      </c>
       <c r="F24">
+        <v>0.73696700000000004</v>
+      </c>
+      <c r="G24">
+        <v>0.68093400000000004</v>
+      </c>
+      <c r="H24">
+        <v>0.59279000000000004</v>
+      </c>
+      <c r="I24">
+        <v>0.46515299999999998</v>
+      </c>
+      <c r="J24">
+        <v>0.38411400000000001</v>
+      </c>
+      <c r="K24">
+        <v>0.311332</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>1000</v>
+      </c>
+      <c r="F25">
+        <v>1000</v>
+      </c>
+      <c r="G25">
+        <v>1000</v>
+      </c>
+      <c r="H25">
+        <v>1000</v>
+      </c>
+      <c r="I25">
+        <v>1000</v>
+      </c>
+      <c r="J25">
+        <v>1000</v>
+      </c>
+      <c r="K25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F33">
         <v>16</v>
       </c>
-      <c r="G24">
+      <c r="G33">
         <v>32</v>
       </c>
-      <c r="H24">
+      <c r="H33">
         <v>64</v>
       </c>
-      <c r="I24">
+      <c r="I33">
         <v>128</v>
       </c>
-      <c r="J24">
+      <c r="J33">
         <v>256</v>
       </c>
-      <c r="K24">
+      <c r="K33">
         <v>512</v>
       </c>
-      <c r="L24">
+      <c r="L33">
         <v>1024</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
-      <c r="F25">
+    <row r="34" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F34">
         <v>0.63151199999999996</v>
       </c>
-      <c r="G25">
+      <c r="G34">
         <v>0.34412399999999999</v>
       </c>
-      <c r="H25">
+      <c r="H34">
         <v>0.20035600000000001</v>
       </c>
-      <c r="I25">
+      <c r="I34">
         <v>0.112299</v>
       </c>
-      <c r="J25">
+      <c r="J34">
         <v>6.7882999999999999E-2</v>
       </c>
-      <c r="K25">
+      <c r="K34">
         <v>4.7099000000000002E-2</v>
       </c>
-      <c r="L25">
+      <c r="L34">
         <v>2.9177999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
-      <c r="E31">
+    <row r="40" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E40">
         <v>0.54377600000000004</v>
       </c>
-      <c r="F31">
+      <c r="F40">
         <v>0.36075000000000002</v>
       </c>
-      <c r="G31">
+      <c r="G40">
         <v>0.21074100000000001</v>
       </c>
-      <c r="H31">
+      <c r="H40">
         <v>9.8393999999999995E-2</v>
       </c>
-      <c r="I31">
+      <c r="I40">
         <v>5.1644000000000002E-2</v>
       </c>
-      <c r="J31">
+      <c r="J40">
         <v>2.648E-2</v>
       </c>
-      <c r="K31">
+      <c r="K40">
         <v>1.4001E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
got dim 0 working with adjacency lists and k_n
</commit_message>
<xml_diff>
--- a/prog1_data.xlsx
+++ b/prog1_data.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emma/Documents/Spring 2016/CS 124/pset3/124pset3/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16460" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24120" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="8">
   <si>
     <t>Dimension</t>
   </si>
@@ -45,6 +40,9 @@
   </si>
   <si>
     <t>0.025+(1.25)*4.53261/(n^0.754872)</t>
+  </si>
+  <si>
+    <t>NEW WITH ADJACENCY LIST</t>
   </si>
 </sst>
 </file>
@@ -112,8 +110,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -164,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -187,6 +189,8 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -209,6 +213,8 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,13 +549,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Q40"/>
+  <dimension ref="A3:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="0.6640625" style="1" customWidth="1"/>
@@ -557,8 +563,8 @@
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1"/>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -608,7 +614,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -633,8 +639,20 @@
       <c r="K5">
         <v>2.1048170000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>1.1981839999999999</v>
+      </c>
+      <c r="M5">
+        <v>1.2074119999999999</v>
+      </c>
+      <c r="N5">
+        <v>1.1969030000000001</v>
+      </c>
+      <c r="O5">
+        <v>1.207155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="D6" t="s">
         <v>3</v>
       </c>
@@ -659,8 +677,20 @@
       <c r="K6">
         <v>1.4001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>4.8900000000000002E-3</v>
+      </c>
+      <c r="M6">
+        <v>2.4239999999999999E-3</v>
+      </c>
+      <c r="N6">
+        <v>1.7780000000000001E-3</v>
+      </c>
+      <c r="O6">
+        <v>6.7699999999999998E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="D7" t="s">
         <v>4</v>
       </c>
@@ -685,8 +715,11 @@
       <c r="K7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="C8" t="s">
         <v>5</v>
       </c>
@@ -722,8 +755,8 @@
         <v>5.5259881066909836E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1"/>
+    <row r="10" spans="1:17">
       <c r="C10">
         <v>2</v>
       </c>
@@ -770,7 +803,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17">
       <c r="D11" t="s">
         <v>2</v>
       </c>
@@ -796,7 +829,7 @@
         <v>21.055610999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17">
       <c r="D12" t="s">
         <v>3</v>
       </c>
@@ -822,7 +855,7 @@
         <v>8.2371E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17">
       <c r="D13" t="s">
         <v>4</v>
       </c>
@@ -848,13 +881,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17">
       <c r="D14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1"/>
+    <row r="16" spans="1:17">
       <c r="C16">
         <v>3</v>
       </c>
@@ -901,7 +934,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17">
       <c r="D17" t="s">
         <v>2</v>
       </c>
@@ -927,7 +960,7 @@
         <v>68.157043000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17">
       <c r="D18" t="s">
         <v>3</v>
       </c>
@@ -953,7 +986,7 @@
         <v>0.21005499999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17">
       <c r="D19" t="s">
         <v>4</v>
       </c>
@@ -979,13 +1012,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17">
       <c r="D20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1"/>
+    <row r="22" spans="1:17">
       <c r="C22">
         <v>4</v>
       </c>
@@ -1032,7 +1065,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17">
       <c r="D23" t="s">
         <v>2</v>
       </c>
@@ -1057,8 +1090,11 @@
       <c r="K23">
         <v>129.93571499999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>1642.5314940000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="D24" t="s">
         <v>3</v>
       </c>
@@ -1083,8 +1119,11 @@
       <c r="K24">
         <v>0.311332</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>1.7208779999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="D25" t="s">
         <v>4</v>
       </c>
@@ -1110,12 +1149,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17">
       <c r="D26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="4" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1134,7 +1173,198 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>32</v>
+      </c>
+      <c r="G28">
+        <v>64</v>
+      </c>
+      <c r="H28">
+        <v>128</v>
+      </c>
+      <c r="I28">
+        <v>256</v>
+      </c>
+      <c r="J28">
+        <v>512</v>
+      </c>
+      <c r="K28">
+        <v>1024</v>
+      </c>
+      <c r="L28">
+        <v>2048</v>
+      </c>
+      <c r="M28">
+        <v>4096</v>
+      </c>
+      <c r="N28">
+        <v>8192</v>
+      </c>
+      <c r="O28">
+        <v>16834</v>
+      </c>
+      <c r="P28">
+        <v>32768</v>
+      </c>
+      <c r="Q28">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>1.3182739999999999</v>
+      </c>
+      <c r="F29">
+        <v>1.481506</v>
+      </c>
+      <c r="G29">
+        <v>1.4887440000000001</v>
+      </c>
+      <c r="H29">
+        <v>1.777309</v>
+      </c>
+      <c r="I29">
+        <v>1.7929740000000001</v>
+      </c>
+      <c r="J29">
+        <v>2.002005</v>
+      </c>
+      <c r="K29">
+        <v>2.1048170000000002</v>
+      </c>
+      <c r="L29">
+        <v>1.1981839999999999</v>
+      </c>
+      <c r="M29">
+        <v>1.2074119999999999</v>
+      </c>
+      <c r="N29">
+        <v>1.1969030000000001</v>
+      </c>
+      <c r="O29">
+        <v>1.207155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>0.54377600000000004</v>
+      </c>
+      <c r="F30">
+        <v>0.36075000000000002</v>
+      </c>
+      <c r="G30">
+        <v>0.21074100000000001</v>
+      </c>
+      <c r="H30">
+        <v>9.8393999999999995E-2</v>
+      </c>
+      <c r="I30">
+        <v>5.1644000000000002E-2</v>
+      </c>
+      <c r="J30">
+        <v>2.648E-2</v>
+      </c>
+      <c r="K30">
+        <v>1.4001E-2</v>
+      </c>
+      <c r="L30">
+        <v>4.8900000000000002E-3</v>
+      </c>
+      <c r="M30">
+        <v>2.4239999999999999E-3</v>
+      </c>
+      <c r="N30">
+        <v>1.7780000000000001E-3</v>
+      </c>
+      <c r="O30">
+        <v>6.7699999999999998E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>10000</v>
+      </c>
+      <c r="F31">
+        <v>10000</v>
+      </c>
+      <c r="G31">
+        <v>10000</v>
+      </c>
+      <c r="H31">
+        <v>1000</v>
+      </c>
+      <c r="I31">
+        <v>1000</v>
+      </c>
+      <c r="J31">
+        <v>1000</v>
+      </c>
+      <c r="K31">
+        <v>1000</v>
+      </c>
+      <c r="O31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <f>0.025+(1.25)*4.53261/POWER(E28,0.754872)</f>
+        <v>0.72371795914248438</v>
+      </c>
+      <c r="F32">
+        <f t="shared" ref="F32:K32" si="1">0.025+(1.25)*4.53261/POWER(F28,0.754872)</f>
+        <v>0.43905953606137094</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>0.27037125053114047</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>0.17040674792789209</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>0.11116788762822982</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>7.6063000611177226E-2</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>5.5259881066909836E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="5:18">
       <c r="F33">
         <v>16</v>
       </c>
@@ -1157,7 +1387,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:18">
       <c r="F34">
         <v>0.63151199999999996</v>
       </c>
@@ -1180,7 +1410,35 @@
         <v>2.9177999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:18">
+      <c r="O38">
+        <v>1.1981839999999999</v>
+      </c>
+      <c r="P38">
+        <v>1.2074119999999999</v>
+      </c>
+      <c r="Q38">
+        <v>1.1969030000000001</v>
+      </c>
+      <c r="R38">
+        <v>1.207155</v>
+      </c>
+    </row>
+    <row r="39" spans="5:18">
+      <c r="O39">
+        <v>4.8900000000000002E-3</v>
+      </c>
+      <c r="P39">
+        <v>2.4239999999999999E-3</v>
+      </c>
+      <c r="Q39">
+        <v>1.7780000000000001E-3</v>
+      </c>
+      <c r="R39">
+        <v>6.7699999999999998E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="5:18">
       <c r="E40">
         <v>0.54377600000000004</v>
       </c>
@@ -1206,5 +1464,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
did k_n for dimensions 2, 3, 4
</commit_message>
<xml_diff>
--- a/prog1_data.xlsx
+++ b/prog1_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24120" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="580" yWindow="0" windowWidth="24120" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,8 +110,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -166,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -191,6 +197,9 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -215,6 +224,9 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -551,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -828,6 +840,9 @@
       <c r="K11">
         <v>21.055610999999999</v>
       </c>
+      <c r="L11">
+        <v>29.667967000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:17">
       <c r="D12" t="s">
@@ -837,7 +852,7 @@
         <v>0.69535599999999997</v>
       </c>
       <c r="F12">
-        <v>0.44828499999999999</v>
+        <v>0.478966</v>
       </c>
       <c r="G12">
         <v>0.352937</v>
@@ -853,6 +868,9 @@
       </c>
       <c r="K12">
         <v>8.2371E-2</v>
+      </c>
+      <c r="L12">
+        <v>6.4424999999999996E-2</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -878,6 +896,9 @@
         <v>1000</v>
       </c>
       <c r="K13">
+        <v>100</v>
+      </c>
+      <c r="L13">
         <v>100</v>
       </c>
     </row>
@@ -1090,9 +1111,6 @@
       <c r="K23">
         <v>129.93571499999999</v>
       </c>
-      <c r="L23">
-        <v>1642.5314940000001</v>
-      </c>
     </row>
     <row r="24" spans="1:17">
       <c r="D24" t="s">
@@ -1118,9 +1136,6 @@
       </c>
       <c r="K24">
         <v>0.311332</v>
-      </c>
-      <c r="L24">
-        <v>1.7208779999999999</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1410,7 +1425,74 @@
         <v>2.9177999999999999E-2</v>
       </c>
     </row>
+    <row r="36" spans="5:18">
+      <c r="E36">
+        <v>0.88619400000000004</v>
+      </c>
+      <c r="F36">
+        <v>0.73696700000000004</v>
+      </c>
+      <c r="G36">
+        <v>0.68093400000000004</v>
+      </c>
+      <c r="H36">
+        <v>0.59279000000000004</v>
+      </c>
+      <c r="I36">
+        <v>0.46515299999999998</v>
+      </c>
+      <c r="J36">
+        <v>0.38411400000000001</v>
+      </c>
+      <c r="K36">
+        <v>0.311332</v>
+      </c>
+    </row>
+    <row r="37" spans="5:18">
+      <c r="E37">
+        <v>0.82371000000000005</v>
+      </c>
+      <c r="F37">
+        <v>0.72728199999999998</v>
+      </c>
+      <c r="G37">
+        <v>0.53383800000000003</v>
+      </c>
+      <c r="H37">
+        <v>0.43611</v>
+      </c>
+      <c r="I37">
+        <v>0.35639900000000002</v>
+      </c>
+      <c r="J37">
+        <v>0.25657000000000002</v>
+      </c>
+      <c r="K37">
+        <v>0.21005499999999999</v>
+      </c>
+    </row>
     <row r="38" spans="5:18">
+      <c r="E38">
+        <v>0.69535599999999997</v>
+      </c>
+      <c r="F38">
+        <v>0.478966</v>
+      </c>
+      <c r="G38">
+        <v>0.352937</v>
+      </c>
+      <c r="H38">
+        <v>0.240012</v>
+      </c>
+      <c r="I38">
+        <v>0.184145</v>
+      </c>
+      <c r="J38">
+        <v>0.13089100000000001</v>
+      </c>
+      <c r="K38">
+        <v>8.2371E-2</v>
+      </c>
       <c r="O38">
         <v>1.1981839999999999</v>
       </c>

</xml_diff>

<commit_message>
dimension 2 data recorded
</commit_message>
<xml_diff>
--- a/prog1_data.xlsx
+++ b/prog1_data.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emma/Documents/Spring 2016/CS 124/pset3/124pset3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="580" yWindow="0" windowWidth="24120" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="1540" yWindow="520" windowWidth="16420" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
   <si>
     <t>Dimension</t>
   </si>
@@ -40,9 +45,6 @@
   </si>
   <si>
     <t>0.025+(1.25)*4.53261/(n^0.754872)</t>
-  </si>
-  <si>
-    <t>NEW WITH ADJACENCY LIST</t>
   </si>
 </sst>
 </file>
@@ -110,18 +112,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -172,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -195,11 +187,6 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -222,11 +209,6 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,13 +543,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:R40"/>
+  <dimension ref="A3:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="0.6640625" style="1" customWidth="1"/>
@@ -575,8 +557,8 @@
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1"/>
-    <row r="4" spans="1:17">
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -626,7 +608,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -652,19 +634,13 @@
         <v>2.1048170000000002</v>
       </c>
       <c r="L5">
-        <v>1.1981839999999999</v>
+        <v>1.2023200000000001</v>
       </c>
       <c r="M5">
-        <v>1.2074119999999999</v>
-      </c>
-      <c r="N5">
-        <v>1.1969030000000001</v>
-      </c>
-      <c r="O5">
-        <v>1.207155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>1.20123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>3</v>
       </c>
@@ -690,19 +666,10 @@
         <v>1.4001E-2</v>
       </c>
       <c r="L6">
-        <v>4.8900000000000002E-3</v>
-      </c>
-      <c r="M6">
-        <v>2.4239999999999999E-3</v>
-      </c>
-      <c r="N6">
-        <v>1.7780000000000001E-3</v>
-      </c>
-      <c r="O6">
-        <v>6.7699999999999998E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>6.5799999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>4</v>
       </c>
@@ -727,11 +694,11 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="O7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="L7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>5</v>
       </c>
@@ -767,8 +734,8 @@
         <v>5.5259881066909836E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1"/>
-    <row r="10" spans="1:17">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>2</v>
       </c>
@@ -815,7 +782,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>2</v>
       </c>
@@ -841,10 +808,25 @@
         <v>21.055610999999999</v>
       </c>
       <c r="L11">
-        <v>29.667967000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>29.677085999999999</v>
+      </c>
+      <c r="M11">
+        <v>41.798164</v>
+      </c>
+      <c r="N11">
+        <v>59.030811</v>
+      </c>
+      <c r="O11">
+        <v>84.327415000000002</v>
+      </c>
+      <c r="P11">
+        <v>117.4776</v>
+      </c>
+      <c r="Q11">
+        <v>166.05796799999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>3</v>
       </c>
@@ -852,7 +834,7 @@
         <v>0.69535599999999997</v>
       </c>
       <c r="F12">
-        <v>0.478966</v>
+        <v>0.44828499999999999</v>
       </c>
       <c r="G12">
         <v>0.352937</v>
@@ -870,10 +852,25 @@
         <v>8.2371E-2</v>
       </c>
       <c r="L12">
-        <v>6.4424999999999996E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>5.8645999999999997E-2</v>
+      </c>
+      <c r="M12">
+        <v>3.3639000000000002E-2</v>
+      </c>
+      <c r="N12">
+        <v>2.2433000000000002E-2</v>
+      </c>
+      <c r="O12">
+        <v>1.5831000000000001E-2</v>
+      </c>
+      <c r="P12">
+        <v>1.4917E-2</v>
+      </c>
+      <c r="Q12">
+        <v>8.6700000000000006E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>4</v>
       </c>
@@ -901,14 +898,29 @@
       <c r="L13">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="M13">
+        <v>10</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
+      </c>
+      <c r="O13">
+        <v>10</v>
+      </c>
+      <c r="P13">
+        <v>5</v>
+      </c>
+      <c r="Q13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1"/>
-    <row r="16" spans="1:17">
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C16">
         <v>3</v>
       </c>
@@ -955,7 +967,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>2</v>
       </c>
@@ -981,7 +993,7 @@
         <v>68.157043000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>3</v>
       </c>
@@ -1007,7 +1019,7 @@
         <v>0.21005499999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>4</v>
       </c>
@@ -1033,13 +1045,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1"/>
-    <row r="22" spans="1:17">
+    <row r="21" spans="1:17" s="1" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C22">
         <v>4</v>
       </c>
@@ -1086,7 +1098,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>2</v>
       </c>
@@ -1112,7 +1124,7 @@
         <v>129.93571499999999</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>3</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>0.311332</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>4</v>
       </c>
@@ -1164,12 +1176,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="4" customHeight="1">
+    <row r="27" spans="1:17" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1188,198 +1200,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>16</v>
-      </c>
-      <c r="F28">
-        <v>32</v>
-      </c>
-      <c r="G28">
-        <v>64</v>
-      </c>
-      <c r="H28">
-        <v>128</v>
-      </c>
-      <c r="I28">
-        <v>256</v>
-      </c>
-      <c r="J28">
-        <v>512</v>
-      </c>
-      <c r="K28">
-        <v>1024</v>
-      </c>
-      <c r="L28">
-        <v>2048</v>
-      </c>
-      <c r="M28">
-        <v>4096</v>
-      </c>
-      <c r="N28">
-        <v>8192</v>
-      </c>
-      <c r="O28">
-        <v>16834</v>
-      </c>
-      <c r="P28">
-        <v>32768</v>
-      </c>
-      <c r="Q28">
-        <v>65536</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="D29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29">
-        <v>1.3182739999999999</v>
-      </c>
-      <c r="F29">
-        <v>1.481506</v>
-      </c>
-      <c r="G29">
-        <v>1.4887440000000001</v>
-      </c>
-      <c r="H29">
-        <v>1.777309</v>
-      </c>
-      <c r="I29">
-        <v>1.7929740000000001</v>
-      </c>
-      <c r="J29">
-        <v>2.002005</v>
-      </c>
-      <c r="K29">
-        <v>2.1048170000000002</v>
-      </c>
-      <c r="L29">
-        <v>1.1981839999999999</v>
-      </c>
-      <c r="M29">
-        <v>1.2074119999999999</v>
-      </c>
-      <c r="N29">
-        <v>1.1969030000000001</v>
-      </c>
-      <c r="O29">
-        <v>1.207155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="D30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30">
-        <v>0.54377600000000004</v>
-      </c>
-      <c r="F30">
-        <v>0.36075000000000002</v>
-      </c>
-      <c r="G30">
-        <v>0.21074100000000001</v>
-      </c>
-      <c r="H30">
-        <v>9.8393999999999995E-2</v>
-      </c>
-      <c r="I30">
-        <v>5.1644000000000002E-2</v>
-      </c>
-      <c r="J30">
-        <v>2.648E-2</v>
-      </c>
-      <c r="K30">
-        <v>1.4001E-2</v>
-      </c>
-      <c r="L30">
-        <v>4.8900000000000002E-3</v>
-      </c>
-      <c r="M30">
-        <v>2.4239999999999999E-3</v>
-      </c>
-      <c r="N30">
-        <v>1.7780000000000001E-3</v>
-      </c>
-      <c r="O30">
-        <v>6.7699999999999998E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="D31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31">
-        <v>10000</v>
-      </c>
-      <c r="F31">
-        <v>10000</v>
-      </c>
-      <c r="G31">
-        <v>10000</v>
-      </c>
-      <c r="H31">
-        <v>1000</v>
-      </c>
-      <c r="I31">
-        <v>1000</v>
-      </c>
-      <c r="J31">
-        <v>1000</v>
-      </c>
-      <c r="K31">
-        <v>1000</v>
-      </c>
-      <c r="O31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32">
-        <f>0.025+(1.25)*4.53261/POWER(E28,0.754872)</f>
-        <v>0.72371795914248438</v>
-      </c>
-      <c r="F32">
-        <f t="shared" ref="F32:K32" si="1">0.025+(1.25)*4.53261/POWER(F28,0.754872)</f>
-        <v>0.43905953606137094</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="1"/>
-        <v>0.27037125053114047</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="1"/>
-        <v>0.17040674792789209</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="1"/>
-        <v>0.11116788762822982</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="1"/>
-        <v>7.6063000611177226E-2</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="1"/>
-        <v>5.5259881066909836E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="5:18">
+    <row r="33" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F33">
         <v>16</v>
       </c>
@@ -1402,7 +1223,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="34" spans="5:18">
+    <row r="34" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F34">
         <v>0.63151199999999996</v>
       </c>
@@ -1425,102 +1246,7 @@
         <v>2.9177999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="5:18">
-      <c r="E36">
-        <v>0.88619400000000004</v>
-      </c>
-      <c r="F36">
-        <v>0.73696700000000004</v>
-      </c>
-      <c r="G36">
-        <v>0.68093400000000004</v>
-      </c>
-      <c r="H36">
-        <v>0.59279000000000004</v>
-      </c>
-      <c r="I36">
-        <v>0.46515299999999998</v>
-      </c>
-      <c r="J36">
-        <v>0.38411400000000001</v>
-      </c>
-      <c r="K36">
-        <v>0.311332</v>
-      </c>
-    </row>
-    <row r="37" spans="5:18">
-      <c r="E37">
-        <v>0.82371000000000005</v>
-      </c>
-      <c r="F37">
-        <v>0.72728199999999998</v>
-      </c>
-      <c r="G37">
-        <v>0.53383800000000003</v>
-      </c>
-      <c r="H37">
-        <v>0.43611</v>
-      </c>
-      <c r="I37">
-        <v>0.35639900000000002</v>
-      </c>
-      <c r="J37">
-        <v>0.25657000000000002</v>
-      </c>
-      <c r="K37">
-        <v>0.21005499999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="5:18">
-      <c r="E38">
-        <v>0.69535599999999997</v>
-      </c>
-      <c r="F38">
-        <v>0.478966</v>
-      </c>
-      <c r="G38">
-        <v>0.352937</v>
-      </c>
-      <c r="H38">
-        <v>0.240012</v>
-      </c>
-      <c r="I38">
-        <v>0.184145</v>
-      </c>
-      <c r="J38">
-        <v>0.13089100000000001</v>
-      </c>
-      <c r="K38">
-        <v>8.2371E-2</v>
-      </c>
-      <c r="O38">
-        <v>1.1981839999999999</v>
-      </c>
-      <c r="P38">
-        <v>1.2074119999999999</v>
-      </c>
-      <c r="Q38">
-        <v>1.1969030000000001</v>
-      </c>
-      <c r="R38">
-        <v>1.207155</v>
-      </c>
-    </row>
-    <row r="39" spans="5:18">
-      <c r="O39">
-        <v>4.8900000000000002E-3</v>
-      </c>
-      <c r="P39">
-        <v>2.4239999999999999E-3</v>
-      </c>
-      <c r="Q39">
-        <v>1.7780000000000001E-3</v>
-      </c>
-      <c r="R39">
-        <v>6.7699999999999998E-4</v>
-      </c>
-    </row>
-    <row r="40" spans="5:18">
+    <row r="40" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E40">
         <v>0.54377600000000004</v>
       </c>
@@ -1546,10 +1272,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added EVEN more values to spreadsheet
</commit_message>
<xml_diff>
--- a/prog1_data.xlsx
+++ b/prog1_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="520" windowWidth="16420" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="16420" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,6 +992,24 @@
       <c r="K17">
         <v>68.157043000000002</v>
       </c>
+      <c r="L17">
+        <v>107.345932</v>
+      </c>
+      <c r="M17">
+        <v>168.68859900000001</v>
+      </c>
+      <c r="N17">
+        <v>266.88738999999998</v>
+      </c>
+      <c r="O17">
+        <v>430.70361300000002</v>
+      </c>
+      <c r="P17">
+        <v>669.03332499999999</v>
+      </c>
+      <c r="Q17">
+        <v>1059.059814</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
@@ -1018,6 +1036,21 @@
       <c r="K18">
         <v>0.21005499999999999</v>
       </c>
+      <c r="L18">
+        <v>0.140599</v>
+      </c>
+      <c r="M18">
+        <v>0.13150600000000001</v>
+      </c>
+      <c r="N18">
+        <v>8.5169999999999996E-2</v>
+      </c>
+      <c r="O18">
+        <v>6.9922999999999999E-2</v>
+      </c>
+      <c r="P18">
+        <v>5.2838000000000003E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
@@ -1043,6 +1076,24 @@
       </c>
       <c r="K19">
         <v>100</v>
+      </c>
+      <c r="L19">
+        <v>10</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19">
+        <v>10</v>
+      </c>
+      <c r="P19">
+        <v>5</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -1123,6 +1174,18 @@
       <c r="K23">
         <v>129.93571499999999</v>
       </c>
+      <c r="L23">
+        <v>216.75732400000001</v>
+      </c>
+      <c r="M23">
+        <v>361.46298200000001</v>
+      </c>
+      <c r="N23">
+        <v>602.69201699999996</v>
+      </c>
+      <c r="O23">
+        <v>1028.2650149999999</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
@@ -1149,6 +1212,18 @@
       <c r="K24">
         <v>0.311332</v>
       </c>
+      <c r="L24">
+        <v>0.243614</v>
+      </c>
+      <c r="M24">
+        <v>0.21598300000000001</v>
+      </c>
+      <c r="N24">
+        <v>0.165379</v>
+      </c>
+      <c r="O24">
+        <v>0.138293</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
@@ -1174,6 +1249,18 @@
       </c>
       <c r="K25">
         <v>100</v>
+      </c>
+      <c r="L25">
+        <v>10</v>
+      </c>
+      <c r="M25">
+        <v>10</v>
+      </c>
+      <c r="N25">
+        <v>10</v>
+      </c>
+      <c r="O25">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
all data filled in
</commit_message>
<xml_diff>
--- a/prog1_data.xlsx
+++ b/prog1_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="16420" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="16420" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,31 +613,43 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <v>1.3182739999999999</v>
+        <v>1.158234</v>
       </c>
       <c r="F5">
-        <v>1.481506</v>
+        <v>1.183538</v>
       </c>
       <c r="G5">
-        <v>1.4887440000000001</v>
+        <v>1.194542</v>
       </c>
       <c r="H5">
-        <v>1.777309</v>
+        <v>1.1993769999999999</v>
       </c>
       <c r="I5">
-        <v>1.7929740000000001</v>
+        <v>1.2029209999999999</v>
       </c>
       <c r="J5">
-        <v>2.002005</v>
+        <v>1.2030639999999999</v>
       </c>
       <c r="K5">
-        <v>2.1048170000000002</v>
+        <v>1.2019660000000001</v>
       </c>
       <c r="L5">
-        <v>1.2023200000000001</v>
+        <v>1.2002759999999999</v>
       </c>
       <c r="M5">
-        <v>1.20123</v>
+        <v>1.198312</v>
+      </c>
+      <c r="N5">
+        <v>1.193554</v>
+      </c>
+      <c r="O5">
+        <v>1.2041850000000001</v>
+      </c>
+      <c r="P5">
+        <v>1.205743</v>
+      </c>
+      <c r="Q5">
+        <v>1.200774</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -645,28 +657,43 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>0.54377600000000004</v>
+        <v>0.55221299999999995</v>
       </c>
       <c r="F6">
-        <v>0.36075000000000002</v>
+        <v>0.35253600000000002</v>
       </c>
       <c r="G6">
-        <v>0.21074100000000001</v>
+        <v>0.21062</v>
       </c>
       <c r="H6">
-        <v>9.8393999999999995E-2</v>
+        <v>0.105326</v>
       </c>
       <c r="I6">
-        <v>5.1644000000000002E-2</v>
+        <v>5.1035999999999998E-2</v>
       </c>
       <c r="J6">
-        <v>2.648E-2</v>
+        <v>2.6724999999999999E-2</v>
       </c>
       <c r="K6">
-        <v>1.4001E-2</v>
+        <v>1.4557E-2</v>
       </c>
       <c r="L6">
-        <v>6.5799999999999999E-3</v>
+        <v>7.0740000000000004E-3</v>
+      </c>
+      <c r="M6">
+        <v>3.225E-3</v>
+      </c>
+      <c r="N6">
+        <v>1.446E-3</v>
+      </c>
+      <c r="O6">
+        <v>7.6499999999999995E-4</v>
+      </c>
+      <c r="P6">
+        <v>4.1100000000000002E-4</v>
+      </c>
+      <c r="Q6">
+        <v>2.0599999999999999E-4</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -683,7 +710,7 @@
         <v>10000</v>
       </c>
       <c r="H7">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="I7">
         <v>1000</v>
@@ -696,6 +723,21 @@
       </c>
       <c r="L7">
         <v>100</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+      <c r="O7">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1186,6 +1228,12 @@
       <c r="O23">
         <v>1028.2650149999999</v>
       </c>
+      <c r="P23">
+        <v>1688.6282960000001</v>
+      </c>
+      <c r="Q23">
+        <v>2830.0883789999998</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
@@ -1224,6 +1272,12 @@
       <c r="O24">
         <v>0.138293</v>
       </c>
+      <c r="P24">
+        <v>0.113422</v>
+      </c>
+      <c r="Q24">
+        <v>0.10422099999999999</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
@@ -1261,6 +1315,12 @@
       </c>
       <c r="O25">
         <v>10</v>
+      </c>
+      <c r="P25">
+        <v>5</v>
+      </c>
+      <c r="Q25">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
all data filled in plus graphs
</commit_message>
<xml_diff>
--- a/prog1_data.xlsx
+++ b/prog1_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="16420" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="25000" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -221,6 +221,3894 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>D</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> = 0</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$Q$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16834.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32768.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65536.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$Q$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.158234</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.183538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.194542</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.199377</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.202921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.203064</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.201966</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.200276</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.198312</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.193554</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.204185</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.205743</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.200774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2093667328"/>
+        <c:axId val="-2131335600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2093667328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2131335600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2131335600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2093667328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>D = 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$Q$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16834.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32768.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65536.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$11:$Q$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.723387</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.869813</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.437021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.611347999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.660027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.981488</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.055611</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.677086</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41.798164</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.030811</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>84.327415</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>117.4776</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>166.057968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2091139360"/>
+        <c:axId val="-2134524432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2091139360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2134524432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2134524432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2091139360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>D = 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$16:$Q$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16834.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32768.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65536.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$17:$Q$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>4.523913</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.162139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.240602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.631735</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.600925</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.319759</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68.157043</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>107.345932</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>168.688599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>266.88739</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>430.703613</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>669.033325</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1059.059814</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2078047312"/>
+        <c:axId val="2134552240"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2078047312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2134552240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2134552240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2078047312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>D = 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0794142607174103"/>
+          <c:y val="0.21337962962963"/>
+          <c:w val="0.838919072615923"/>
+          <c:h val="0.700054316127151"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$22:$Q$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16834.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32768.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65536.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$23:$Q$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.13595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.339508</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.126459</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.387136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.187328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.17495700000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>129.935715</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>216.757324</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>361.462982</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>602.692017</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1028.265015</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1688.628296</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2830.088379</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2111708560"/>
+        <c:axId val="-2090555280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2111708560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2090555280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2090555280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2111708560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -545,8 +4433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="P44" sqref="P44:P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1419,5 +5307,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>